<commit_message>
fix jurisdiction variable in R v. Boutilier
</commit_message>
<xml_diff>
--- a/jr_data.xlsx
+++ b/jr_data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylanclarke/Dropbox/papers/irwintoy/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A2DC37-358E-0849-8AA8-DC7BD40FA230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBA997B-AFC4-E844-A4F0-7192F89B2403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23880" windowHeight="16940" activeTab="1" xr2:uid="{E47A3FDC-7AD1-4511-9448-90402246D381}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23880" windowHeight="16940" xr2:uid="{E47A3FDC-7AD1-4511-9448-90402246D381}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="1" r:id="rId1"/>
     <sheet name="Justice" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7255" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7256" uniqueCount="647">
   <si>
     <t>case</t>
   </si>
@@ -2062,9 +2063,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2102,7 +2103,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2208,7 +2209,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2350,7 +2351,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2360,9 +2361,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC629BE-A775-4F8E-9F9C-1908E990AD15}">
   <dimension ref="A1:J251"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E226" sqref="E226"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3159,6 +3160,9 @@
       <c r="D25" t="s">
         <v>81</v>
       </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
       <c r="F25">
         <v>0</v>
       </c>
@@ -10417,7 +10421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D51641C-C0B7-473D-8C49-9727ECB88893}">
   <dimension ref="A1:I1997"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1782" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1793" sqref="C1793"/>
     </sheetView>

</xml_diff>